<commit_message>
TESI SPA - MEDICAL REPORT - Correzione report-checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/MEDICAL REPORT/1.3/MEDICAL_REPORT_accreditamento-checklist_V8.2.6.1.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/MEDICAL REPORT/1.3/MEDICAL_REPORT_accreditamento-checklist_V8.2.6.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\MEDICAL_REPORT\_TEST_CASES\20250919\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TESI\Bugs\FSE2_0\Accreditamento\MEDICAL_REPORT\_TEST_CASES\20250923\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5768406A-0C30-4CFA-9A59-A648F7C22BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9717621B-2C63-4EF1-8F62-1EC81A398690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="518">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2460,7 +2460,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2580,6 +2580,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2601,33 +2616,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4081,10 +4069,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4126,12 +4114,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="53"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4152,14 +4140,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="61" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="53"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4180,12 +4168,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="56" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="61" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4207,12 +4195,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56" t="s">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4233,8 +4221,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -4521,48 +4509,54 @@
       <c r="A14" s="35">
         <v>31</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="37">
         <v>45890</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="37" t="s">
         <v>440</v>
       </c>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="37" t="s">
         <v>441</v>
       </c>
-      <c r="I14" s="60" t="s">
+      <c r="I14" s="42" t="s">
         <v>442</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59" t="s">
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N14" s="59" t="s">
+      <c r="N14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O14" s="59" t="s">
+      <c r="O14" s="38" t="s">
         <v>443</v>
       </c>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="59"/>
-      <c r="S14" s="59" t="s">
+      <c r="P14" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R14" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S14" s="38" t="s">
         <v>444</v>
       </c>
       <c r="T14" s="38"/>
@@ -4576,48 +4570,54 @@
       <c r="A15" s="35">
         <v>32</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="37">
         <v>45890</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="37" t="s">
         <v>487</v>
       </c>
-      <c r="I15" s="60" t="s">
+      <c r="I15" s="42" t="s">
         <v>442</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="J15" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59" t="s">
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N15" s="59" t="s">
+      <c r="N15" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="O15" s="38" t="s">
         <v>443</v>
       </c>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59" t="s">
+      <c r="P15" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R15" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S15" s="38" t="s">
         <v>444</v>
       </c>
       <c r="T15" s="38"/>
@@ -4853,48 +4853,54 @@
       <c r="A22" s="35">
         <v>39</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="58">
+      <c r="F22" s="37">
         <v>45890</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="37" t="s">
         <v>445</v>
       </c>
-      <c r="H22" s="58" t="s">
+      <c r="H22" s="37" t="s">
         <v>446</v>
       </c>
-      <c r="I22" s="60" t="s">
+      <c r="I22" s="42" t="s">
         <v>442</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59" t="s">
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N22" s="59" t="s">
+      <c r="N22" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O22" s="59" t="s">
+      <c r="O22" s="38" t="s">
         <v>447</v>
       </c>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59" t="s">
+      <c r="P22" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q22" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R22" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S22" s="38" t="s">
         <v>448</v>
       </c>
       <c r="T22" s="38"/>
@@ -4908,48 +4914,54 @@
       <c r="A23" s="35">
         <v>40</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="37">
         <v>45890</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="37" t="s">
         <v>488</v>
       </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="37" t="s">
         <v>489</v>
       </c>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="42" t="s">
         <v>442</v>
       </c>
-      <c r="J23" s="59" t="s">
+      <c r="J23" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59" t="s">
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N23" s="59" t="s">
+      <c r="N23" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O23" s="59" t="s">
+      <c r="O23" s="38" t="s">
         <v>447</v>
       </c>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59" t="s">
+      <c r="P23" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q23" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="R23" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23" s="38" t="s">
         <v>448</v>
       </c>
       <c r="T23" s="38"/>
@@ -5191,48 +5203,48 @@
       <c r="A30" s="35">
         <v>47</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="65" t="s">
+      <c r="E30" s="49" t="s">
         <v>432</v>
       </c>
-      <c r="F30" s="58">
+      <c r="F30" s="37">
         <v>45890</v>
       </c>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="59" t="s">
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59" t="s">
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N30" s="59" t="s">
+      <c r="N30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="59" t="s">
+      <c r="O30" s="38" t="s">
         <v>449</v>
       </c>
-      <c r="P30" s="59" t="s">
+      <c r="P30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q30" s="59" t="s">
+      <c r="Q30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="R30" s="59" t="s">
+      <c r="R30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S30" s="59" t="s">
+      <c r="S30" s="38" t="s">
         <v>450</v>
       </c>
       <c r="T30" s="38"/>
@@ -5248,48 +5260,48 @@
       <c r="A31" s="35">
         <v>48</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E31" s="49" t="s">
         <v>432</v>
       </c>
-      <c r="F31" s="58">
+      <c r="F31" s="37">
         <v>45888</v>
       </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="59" t="s">
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59" t="s">
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N31" s="59" t="s">
+      <c r="N31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="59" t="s">
+      <c r="O31" s="38" t="s">
         <v>449</v>
       </c>
-      <c r="P31" s="59" t="s">
+      <c r="P31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q31" s="59" t="s">
+      <c r="Q31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="R31" s="59" t="s">
+      <c r="R31" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S31" s="59" t="s">
+      <c r="S31" s="38" t="s">
         <v>450</v>
       </c>
       <c r="T31" s="38"/>
@@ -6088,38 +6100,38 @@
       <c r="A53" s="35">
         <v>76</v>
       </c>
-      <c r="B53" s="63" t="s">
+      <c r="B53" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="C53" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="63" t="s">
+      <c r="D53" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="65" t="s">
+      <c r="E53" s="49" t="s">
         <v>299</v>
       </c>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="60"/>
-      <c r="J53" s="59" t="s">
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K53" s="59" t="s">
+      <c r="K53" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L53" s="59" t="s">
+      <c r="L53" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="M53" s="59"/>
-      <c r="N53" s="59"/>
-      <c r="O53" s="59"/>
-      <c r="P53" s="59"/>
-      <c r="Q53" s="59"/>
-      <c r="R53" s="59"/>
-      <c r="S53" s="59"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="38"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="38"/>
+      <c r="R53" s="38"/>
+      <c r="S53" s="38"/>
       <c r="T53" s="38"/>
       <c r="U53" s="39"/>
       <c r="V53" s="40"/>
@@ -6131,38 +6143,38 @@
       <c r="A54" s="35">
         <v>78</v>
       </c>
-      <c r="B54" s="63" t="s">
+      <c r="B54" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="C54" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="63" t="s">
+      <c r="D54" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E54" s="65" t="s">
+      <c r="E54" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="60"/>
-      <c r="J54" s="59" t="s">
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K54" s="59" t="s">
+      <c r="K54" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L54" s="59" t="s">
+      <c r="L54" s="38" t="s">
         <v>452</v>
       </c>
-      <c r="M54" s="59"/>
-      <c r="N54" s="59"/>
-      <c r="O54" s="59"/>
-      <c r="P54" s="59"/>
-      <c r="Q54" s="59"/>
-      <c r="R54" s="59"/>
-      <c r="S54" s="59"/>
+      <c r="M54" s="38"/>
+      <c r="N54" s="38"/>
+      <c r="O54" s="38"/>
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38"/>
+      <c r="R54" s="38"/>
+      <c r="S54" s="38"/>
       <c r="T54" s="38"/>
       <c r="U54" s="39"/>
       <c r="V54" s="40"/>
@@ -6174,38 +6186,38 @@
       <c r="A55" s="35">
         <v>79</v>
       </c>
-      <c r="B55" s="63" t="s">
+      <c r="B55" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="64" t="s">
+      <c r="C55" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D55" s="63" t="s">
+      <c r="D55" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="E55" s="65" t="s">
+      <c r="E55" s="49" t="s">
         <v>300</v>
       </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="59" t="s">
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K55" s="59" t="s">
+      <c r="K55" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L55" s="59" t="s">
+      <c r="L55" s="38" t="s">
         <v>453</v>
       </c>
-      <c r="M55" s="59"/>
-      <c r="N55" s="59"/>
-      <c r="O55" s="59"/>
-      <c r="P55" s="59"/>
-      <c r="Q55" s="59"/>
-      <c r="R55" s="59"/>
-      <c r="S55" s="59"/>
+      <c r="M55" s="38"/>
+      <c r="N55" s="38"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+      <c r="S55" s="38"/>
       <c r="T55" s="38"/>
       <c r="U55" s="39"/>
       <c r="V55" s="40"/>
@@ -6217,38 +6229,38 @@
       <c r="A56" s="35">
         <v>80</v>
       </c>
-      <c r="B56" s="63" t="s">
+      <c r="B56" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="64" t="s">
+      <c r="C56" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="63" t="s">
+      <c r="D56" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="E56" s="65" t="s">
+      <c r="E56" s="49" t="s">
         <v>301</v>
       </c>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="60"/>
-      <c r="J56" s="59" t="s">
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="42"/>
+      <c r="J56" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K56" s="59" t="s">
+      <c r="K56" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L56" s="59" t="s">
+      <c r="L56" s="38" t="s">
         <v>454</v>
       </c>
-      <c r="M56" s="59"/>
-      <c r="N56" s="59"/>
-      <c r="O56" s="59"/>
-      <c r="P56" s="59"/>
-      <c r="Q56" s="59"/>
-      <c r="R56" s="59"/>
-      <c r="S56" s="59"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="38"/>
+      <c r="P56" s="38"/>
+      <c r="Q56" s="38"/>
+      <c r="R56" s="38"/>
+      <c r="S56" s="38"/>
       <c r="T56" s="38"/>
       <c r="U56" s="39"/>
       <c r="V56" s="40"/>
@@ -6260,38 +6272,38 @@
       <c r="A57" s="35">
         <v>81</v>
       </c>
-      <c r="B57" s="63" t="s">
+      <c r="B57" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="64" t="s">
+      <c r="C57" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D57" s="63" t="s">
+      <c r="D57" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="E57" s="65" t="s">
+      <c r="E57" s="49" t="s">
         <v>302</v>
       </c>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="59" t="s">
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K57" s="59" t="s">
+      <c r="K57" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L57" s="59" t="s">
+      <c r="L57" s="38" t="s">
         <v>455</v>
       </c>
-      <c r="M57" s="59"/>
-      <c r="N57" s="59"/>
-      <c r="O57" s="59"/>
-      <c r="P57" s="59"/>
-      <c r="Q57" s="59"/>
-      <c r="R57" s="59"/>
-      <c r="S57" s="59"/>
+      <c r="M57" s="38"/>
+      <c r="N57" s="38"/>
+      <c r="O57" s="38"/>
+      <c r="P57" s="38"/>
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
+      <c r="S57" s="38"/>
       <c r="T57" s="38"/>
       <c r="U57" s="39"/>
       <c r="V57" s="40"/>
@@ -6303,38 +6315,38 @@
       <c r="A58" s="35">
         <v>83</v>
       </c>
-      <c r="B58" s="63" t="s">
+      <c r="B58" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="C58" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="63" t="s">
+      <c r="D58" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="E58" s="65" t="s">
+      <c r="E58" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="60"/>
-      <c r="J58" s="59" t="s">
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K58" s="59" t="s">
+      <c r="K58" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L58" s="59" t="s">
+      <c r="L58" s="38" t="s">
         <v>456</v>
       </c>
-      <c r="M58" s="59"/>
-      <c r="N58" s="59"/>
-      <c r="O58" s="59"/>
-      <c r="P58" s="59"/>
-      <c r="Q58" s="59"/>
-      <c r="R58" s="59"/>
-      <c r="S58" s="59"/>
+      <c r="M58" s="38"/>
+      <c r="N58" s="38"/>
+      <c r="O58" s="38"/>
+      <c r="P58" s="38"/>
+      <c r="Q58" s="38"/>
+      <c r="R58" s="38"/>
+      <c r="S58" s="38"/>
       <c r="T58" s="38"/>
       <c r="U58" s="39"/>
       <c r="V58" s="40"/>
@@ -6346,54 +6358,54 @@
       <c r="A59" s="35">
         <v>84</v>
       </c>
-      <c r="B59" s="63" t="s">
+      <c r="B59" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="64" t="s">
+      <c r="C59" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="63" t="s">
+      <c r="D59" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E59" s="65" t="s">
+      <c r="E59" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="58">
+      <c r="F59" s="37">
         <v>45911</v>
       </c>
-      <c r="G59" s="58" t="s">
+      <c r="G59" s="37" t="s">
         <v>457</v>
       </c>
-      <c r="H59" s="58" t="s">
+      <c r="H59" s="37" t="s">
         <v>458</v>
       </c>
-      <c r="I59" s="60" t="s">
+      <c r="I59" s="42" t="s">
         <v>459</v>
       </c>
-      <c r="J59" s="59" t="s">
+      <c r="J59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K59" s="59"/>
-      <c r="L59" s="59"/>
-      <c r="M59" s="59" t="s">
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
+      <c r="M59" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N59" s="59" t="s">
+      <c r="N59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O59" s="59" t="s">
+      <c r="O59" s="38" t="s">
         <v>460</v>
       </c>
-      <c r="P59" s="59" t="s">
+      <c r="P59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q59" s="59" t="s">
+      <c r="Q59" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R59" s="59" t="s">
+      <c r="R59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S59" s="59" t="s">
+      <c r="S59" s="38" t="s">
         <v>461</v>
       </c>
       <c r="T59" s="38"/>
@@ -6407,38 +6419,38 @@
       <c r="A60" s="35">
         <v>85</v>
       </c>
-      <c r="B60" s="63" t="s">
+      <c r="B60" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="64" t="s">
+      <c r="C60" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="E60" s="65" t="s">
+      <c r="E60" s="49" t="s">
         <v>303</v>
       </c>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="59" t="s">
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="42"/>
+      <c r="J60" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K60" s="59" t="s">
+      <c r="K60" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L60" s="59" t="s">
+      <c r="L60" s="38" t="s">
         <v>462</v>
       </c>
-      <c r="M60" s="59"/>
-      <c r="N60" s="59"/>
-      <c r="O60" s="59"/>
-      <c r="P60" s="59"/>
-      <c r="Q60" s="59"/>
-      <c r="R60" s="59"/>
-      <c r="S60" s="59"/>
+      <c r="M60" s="38"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="38"/>
+      <c r="Q60" s="38"/>
+      <c r="R60" s="38"/>
+      <c r="S60" s="38"/>
       <c r="T60" s="38"/>
       <c r="U60" s="39"/>
       <c r="V60" s="40"/>
@@ -6450,38 +6462,38 @@
       <c r="A61" s="35">
         <v>86</v>
       </c>
-      <c r="B61" s="63" t="s">
+      <c r="B61" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C61" s="64" t="s">
+      <c r="C61" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D61" s="63" t="s">
+      <c r="D61" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="E61" s="65" t="s">
+      <c r="E61" s="49" t="s">
         <v>304</v>
       </c>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="59" t="s">
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="42"/>
+      <c r="J61" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K61" s="59" t="s">
+      <c r="K61" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L61" s="59" t="s">
+      <c r="L61" s="38" t="s">
         <v>463</v>
       </c>
-      <c r="M61" s="59"/>
-      <c r="N61" s="59"/>
-      <c r="O61" s="59"/>
-      <c r="P61" s="59"/>
-      <c r="Q61" s="59"/>
-      <c r="R61" s="59"/>
-      <c r="S61" s="59"/>
+      <c r="M61" s="38"/>
+      <c r="N61" s="38"/>
+      <c r="O61" s="38"/>
+      <c r="P61" s="38"/>
+      <c r="Q61" s="38"/>
+      <c r="R61" s="38"/>
+      <c r="S61" s="38"/>
       <c r="T61" s="38"/>
       <c r="U61" s="39"/>
       <c r="V61" s="40"/>
@@ -6493,38 +6505,38 @@
       <c r="A62" s="35">
         <v>87</v>
       </c>
-      <c r="B62" s="63" t="s">
+      <c r="B62" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="64" t="s">
+      <c r="C62" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D62" s="63" t="s">
+      <c r="D62" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="E62" s="65" t="s">
+      <c r="E62" s="49" t="s">
         <v>305</v>
       </c>
-      <c r="F62" s="58"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="60"/>
-      <c r="J62" s="59" t="s">
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="42"/>
+      <c r="J62" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K62" s="59" t="s">
+      <c r="K62" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L62" s="59" t="s">
+      <c r="L62" s="38" t="s">
         <v>464</v>
       </c>
-      <c r="M62" s="59"/>
-      <c r="N62" s="59"/>
-      <c r="O62" s="59"/>
-      <c r="P62" s="59"/>
-      <c r="Q62" s="59"/>
-      <c r="R62" s="59"/>
-      <c r="S62" s="59"/>
+      <c r="M62" s="38"/>
+      <c r="N62" s="38"/>
+      <c r="O62" s="38"/>
+      <c r="P62" s="38"/>
+      <c r="Q62" s="38"/>
+      <c r="R62" s="38"/>
+      <c r="S62" s="38"/>
       <c r="T62" s="38"/>
       <c r="U62" s="39"/>
       <c r="V62" s="40"/>
@@ -6536,38 +6548,38 @@
       <c r="A63" s="35">
         <v>88</v>
       </c>
-      <c r="B63" s="63" t="s">
+      <c r="B63" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D63" s="63" t="s">
+      <c r="D63" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="E63" s="65" t="s">
+      <c r="E63" s="49" t="s">
         <v>306</v>
       </c>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="60"/>
-      <c r="J63" s="59" t="s">
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="42"/>
+      <c r="J63" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K63" s="59" t="s">
+      <c r="K63" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L63" s="59" t="s">
+      <c r="L63" s="38" t="s">
         <v>465</v>
       </c>
-      <c r="M63" s="59"/>
-      <c r="N63" s="59"/>
-      <c r="O63" s="59"/>
-      <c r="P63" s="59"/>
-      <c r="Q63" s="59"/>
-      <c r="R63" s="59"/>
-      <c r="S63" s="59"/>
+      <c r="M63" s="38"/>
+      <c r="N63" s="38"/>
+      <c r="O63" s="38"/>
+      <c r="P63" s="38"/>
+      <c r="Q63" s="38"/>
+      <c r="R63" s="38"/>
+      <c r="S63" s="38"/>
       <c r="T63" s="38"/>
       <c r="U63" s="39"/>
       <c r="V63" s="40"/>
@@ -6579,54 +6591,54 @@
       <c r="A64" s="35">
         <v>89</v>
       </c>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="64" t="s">
+      <c r="C64" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D64" s="63" t="s">
+      <c r="D64" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="65" t="s">
+      <c r="E64" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="F64" s="58">
+      <c r="F64" s="37">
         <v>45912</v>
       </c>
-      <c r="G64" s="58" t="s">
+      <c r="G64" s="37" t="s">
         <v>466</v>
       </c>
-      <c r="H64" s="58" t="s">
+      <c r="H64" s="37" t="s">
         <v>467</v>
       </c>
-      <c r="I64" s="60" t="s">
+      <c r="I64" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="J64" s="59" t="s">
+      <c r="J64" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K64" s="59"/>
-      <c r="L64" s="59"/>
-      <c r="M64" s="59" t="s">
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N64" s="59" t="s">
+      <c r="N64" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O64" s="59" t="s">
+      <c r="O64" s="38" t="s">
         <v>469</v>
       </c>
-      <c r="P64" s="59" t="s">
+      <c r="P64" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q64" s="59" t="s">
+      <c r="Q64" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R64" s="59" t="s">
+      <c r="R64" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S64" s="59" t="s">
+      <c r="S64" s="38" t="s">
         <v>470</v>
       </c>
       <c r="T64" s="38"/>
@@ -6640,54 +6652,54 @@
       <c r="A65" s="35">
         <v>90</v>
       </c>
-      <c r="B65" s="63" t="s">
+      <c r="B65" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C65" s="64" t="s">
+      <c r="C65" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E65" s="65" t="s">
+      <c r="E65" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F65" s="58">
+      <c r="F65" s="37">
         <v>45912</v>
       </c>
-      <c r="G65" s="58" t="s">
+      <c r="G65" s="37" t="s">
         <v>471</v>
       </c>
-      <c r="H65" s="58" t="s">
+      <c r="H65" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="I65" s="60" t="s">
+      <c r="I65" s="42" t="s">
         <v>473</v>
       </c>
-      <c r="J65" s="59" t="s">
+      <c r="J65" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K65" s="59"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="59" t="s">
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
+      <c r="M65" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N65" s="59" t="s">
+      <c r="N65" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O65" s="59" t="s">
+      <c r="O65" s="38" t="s">
         <v>474</v>
       </c>
-      <c r="P65" s="59" t="s">
+      <c r="P65" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q65" s="59" t="s">
+      <c r="Q65" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R65" s="59" t="s">
+      <c r="R65" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S65" s="59" t="s">
+      <c r="S65" s="38" t="s">
         <v>470</v>
       </c>
       <c r="T65" s="38"/>
@@ -6701,38 +6713,38 @@
       <c r="A66" s="35">
         <v>91</v>
       </c>
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="64" t="s">
+      <c r="C66" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="63" t="s">
+      <c r="D66" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="65" t="s">
+      <c r="E66" s="49" t="s">
         <v>307</v>
       </c>
-      <c r="F66" s="58"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="58"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="59" t="s">
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K66" s="59" t="s">
+      <c r="K66" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L66" s="59" t="s">
+      <c r="L66" s="38" t="s">
         <v>475</v>
       </c>
-      <c r="M66" s="59"/>
-      <c r="N66" s="59"/>
-      <c r="O66" s="59"/>
-      <c r="P66" s="59"/>
-      <c r="Q66" s="59"/>
-      <c r="R66" s="59"/>
-      <c r="S66" s="59"/>
+      <c r="M66" s="38"/>
+      <c r="N66" s="38"/>
+      <c r="O66" s="38"/>
+      <c r="P66" s="38"/>
+      <c r="Q66" s="38"/>
+      <c r="R66" s="38"/>
+      <c r="S66" s="38"/>
       <c r="T66" s="38"/>
       <c r="U66" s="39"/>
       <c r="V66" s="40"/>
@@ -6744,52 +6756,54 @@
       <c r="A67" s="35">
         <v>92</v>
       </c>
-      <c r="B67" s="63" t="s">
+      <c r="B67" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C67" s="64" t="s">
+      <c r="C67" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="63" t="s">
+      <c r="D67" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="E67" s="65" t="s">
+      <c r="E67" s="49" t="s">
         <v>356</v>
       </c>
-      <c r="F67" s="58">
+      <c r="F67" s="37">
         <v>45912</v>
       </c>
-      <c r="G67" s="58" t="s">
+      <c r="G67" s="37" t="s">
         <v>476</v>
       </c>
-      <c r="H67" s="58" t="s">
+      <c r="H67" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="I67" s="60" t="s">
+      <c r="I67" s="42" t="s">
         <v>478</v>
       </c>
-      <c r="J67" s="59"/>
-      <c r="K67" s="59"/>
-      <c r="L67" s="59"/>
-      <c r="M67" s="59" t="s">
+      <c r="J67" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
+      <c r="M67" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N67" s="59" t="s">
+      <c r="N67" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O67" s="59" t="s">
+      <c r="O67" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="P67" s="59" t="s">
+      <c r="P67" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q67" s="59" t="s">
+      <c r="Q67" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R67" s="59" t="s">
+      <c r="R67" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S67" s="59" t="s">
+      <c r="S67" s="38" t="s">
         <v>480</v>
       </c>
       <c r="T67" s="38"/>
@@ -6803,38 +6817,38 @@
       <c r="A68" s="35">
         <v>93</v>
       </c>
-      <c r="B68" s="63" t="s">
+      <c r="B68" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D68" s="63" t="s">
+      <c r="D68" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="E68" s="65" t="s">
+      <c r="E68" s="49" t="s">
         <v>308</v>
       </c>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="60"/>
-      <c r="J68" s="59" t="s">
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="42"/>
+      <c r="J68" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K68" s="59" t="s">
+      <c r="K68" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L68" s="59" t="s">
+      <c r="L68" s="38" t="s">
         <v>481</v>
       </c>
-      <c r="M68" s="59"/>
-      <c r="N68" s="59"/>
-      <c r="O68" s="59"/>
-      <c r="P68" s="59"/>
-      <c r="Q68" s="59"/>
-      <c r="R68" s="59"/>
-      <c r="S68" s="59"/>
+      <c r="M68" s="38"/>
+      <c r="N68" s="38"/>
+      <c r="O68" s="38"/>
+      <c r="P68" s="38"/>
+      <c r="Q68" s="38"/>
+      <c r="R68" s="38"/>
+      <c r="S68" s="38"/>
       <c r="T68" s="38"/>
       <c r="U68" s="39"/>
       <c r="V68" s="40"/>
@@ -7841,7 +7855,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>127</v>
       </c>
@@ -7878,7 +7892,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>128</v>
       </c>
@@ -7915,7 +7929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>129</v>
       </c>
@@ -7952,7 +7966,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>130</v>
       </c>
@@ -7989,7 +8003,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>131</v>
       </c>
@@ -8026,7 +8040,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>132</v>
       </c>
@@ -8063,7 +8077,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>133</v>
       </c>
@@ -8100,7 +8114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>134</v>
       </c>
@@ -8137,7 +8151,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>135</v>
       </c>
@@ -8174,7 +8188,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>136</v>
       </c>
@@ -8211,7 +8225,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>137</v>
       </c>
@@ -8248,7 +8262,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>138</v>
       </c>
@@ -8285,7 +8299,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>139</v>
       </c>
@@ -8322,7 +8336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>140</v>
       </c>
@@ -8359,7 +8373,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>141</v>
       </c>
@@ -8396,7 +8410,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>142</v>
       </c>
@@ -8433,7 +8447,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>143</v>
       </c>
@@ -8470,7 +8484,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>144</v>
       </c>
@@ -8507,7 +8521,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>145</v>
       </c>
@@ -8544,7 +8558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>146</v>
       </c>
@@ -8585,38 +8599,38 @@
       <c r="A116" s="35">
         <v>152</v>
       </c>
-      <c r="B116" s="63" t="s">
+      <c r="B116" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C116" s="64" t="s">
+      <c r="C116" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D116" s="63" t="s">
+      <c r="D116" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="E116" s="65" t="s">
+      <c r="E116" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="F116" s="58"/>
-      <c r="G116" s="58"/>
-      <c r="H116" s="58"/>
-      <c r="I116" s="60"/>
-      <c r="J116" s="59" t="s">
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="42"/>
+      <c r="J116" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K116" s="59" t="s">
+      <c r="K116" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L116" s="59" t="s">
+      <c r="L116" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="M116" s="59"/>
-      <c r="N116" s="59"/>
-      <c r="O116" s="59"/>
-      <c r="P116" s="59"/>
-      <c r="Q116" s="59"/>
-      <c r="R116" s="59"/>
-      <c r="S116" s="59"/>
+      <c r="M116" s="38"/>
+      <c r="N116" s="38"/>
+      <c r="O116" s="38"/>
+      <c r="P116" s="38"/>
+      <c r="Q116" s="38"/>
+      <c r="R116" s="38"/>
+      <c r="S116" s="38"/>
       <c r="T116" s="38"/>
       <c r="U116" s="39"/>
       <c r="V116" s="40"/>
@@ -8628,38 +8642,38 @@
       <c r="A117" s="35">
         <v>154</v>
       </c>
-      <c r="B117" s="63" t="s">
+      <c r="B117" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C117" s="64" t="s">
+      <c r="C117" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D117" s="63" t="s">
+      <c r="D117" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="E117" s="65" t="s">
+      <c r="E117" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="F117" s="58"/>
-      <c r="G117" s="58"/>
-      <c r="H117" s="58"/>
-      <c r="I117" s="60"/>
-      <c r="J117" s="59" t="s">
+      <c r="F117" s="37"/>
+      <c r="G117" s="37"/>
+      <c r="H117" s="37"/>
+      <c r="I117" s="42"/>
+      <c r="J117" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K117" s="59" t="s">
+      <c r="K117" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L117" s="59" t="s">
+      <c r="L117" s="38" t="s">
         <v>452</v>
       </c>
-      <c r="M117" s="59"/>
-      <c r="N117" s="59"/>
-      <c r="O117" s="59"/>
-      <c r="P117" s="59"/>
-      <c r="Q117" s="59"/>
-      <c r="R117" s="59"/>
-      <c r="S117" s="59"/>
+      <c r="M117" s="38"/>
+      <c r="N117" s="38"/>
+      <c r="O117" s="38"/>
+      <c r="P117" s="38"/>
+      <c r="Q117" s="38"/>
+      <c r="R117" s="38"/>
+      <c r="S117" s="38"/>
       <c r="T117" s="38"/>
       <c r="U117" s="39"/>
       <c r="V117" s="40"/>
@@ -8671,38 +8685,38 @@
       <c r="A118" s="35">
         <v>155</v>
       </c>
-      <c r="B118" s="63" t="s">
+      <c r="B118" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C118" s="64" t="s">
+      <c r="C118" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D118" s="63" t="s">
+      <c r="D118" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="E118" s="65" t="s">
+      <c r="E118" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="F118" s="58"/>
-      <c r="G118" s="58"/>
-      <c r="H118" s="58"/>
-      <c r="I118" s="60"/>
-      <c r="J118" s="59" t="s">
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="42"/>
+      <c r="J118" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K118" s="59" t="s">
+      <c r="K118" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L118" s="59" t="s">
+      <c r="L118" s="38" t="s">
         <v>453</v>
       </c>
-      <c r="M118" s="59"/>
-      <c r="N118" s="59"/>
-      <c r="O118" s="59"/>
-      <c r="P118" s="59"/>
-      <c r="Q118" s="59"/>
-      <c r="R118" s="59"/>
-      <c r="S118" s="59"/>
+      <c r="M118" s="38"/>
+      <c r="N118" s="38"/>
+      <c r="O118" s="38"/>
+      <c r="P118" s="38"/>
+      <c r="Q118" s="38"/>
+      <c r="R118" s="38"/>
+      <c r="S118" s="38"/>
       <c r="T118" s="38"/>
       <c r="U118" s="39"/>
       <c r="V118" s="40"/>
@@ -8714,38 +8728,38 @@
       <c r="A119" s="35">
         <v>156</v>
       </c>
-      <c r="B119" s="63" t="s">
+      <c r="B119" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C119" s="64" t="s">
+      <c r="C119" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D119" s="63" t="s">
+      <c r="D119" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="E119" s="65" t="s">
+      <c r="E119" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="F119" s="58"/>
-      <c r="G119" s="58"/>
-      <c r="H119" s="58"/>
-      <c r="I119" s="60"/>
-      <c r="J119" s="59" t="s">
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="42"/>
+      <c r="J119" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K119" s="59" t="s">
+      <c r="K119" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L119" s="59" t="s">
+      <c r="L119" s="38" t="s">
         <v>454</v>
       </c>
-      <c r="M119" s="59"/>
-      <c r="N119" s="59"/>
-      <c r="O119" s="59"/>
-      <c r="P119" s="59"/>
-      <c r="Q119" s="59"/>
-      <c r="R119" s="59"/>
-      <c r="S119" s="59"/>
+      <c r="M119" s="38"/>
+      <c r="N119" s="38"/>
+      <c r="O119" s="38"/>
+      <c r="P119" s="38"/>
+      <c r="Q119" s="38"/>
+      <c r="R119" s="38"/>
+      <c r="S119" s="38"/>
       <c r="T119" s="38"/>
       <c r="U119" s="39"/>
       <c r="V119" s="40"/>
@@ -8757,38 +8771,38 @@
       <c r="A120" s="35">
         <v>159</v>
       </c>
-      <c r="B120" s="63" t="s">
+      <c r="B120" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C120" s="64" t="s">
+      <c r="C120" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D120" s="63" t="s">
+      <c r="D120" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="E120" s="65" t="s">
+      <c r="E120" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="F120" s="58"/>
-      <c r="G120" s="58"/>
-      <c r="H120" s="58"/>
-      <c r="I120" s="60"/>
-      <c r="J120" s="59" t="s">
+      <c r="F120" s="37"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="42"/>
+      <c r="J120" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K120" s="59" t="s">
+      <c r="K120" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L120" s="59" t="s">
+      <c r="L120" s="38" t="s">
         <v>456</v>
       </c>
-      <c r="M120" s="59"/>
-      <c r="N120" s="59"/>
-      <c r="O120" s="59"/>
-      <c r="P120" s="59"/>
-      <c r="Q120" s="59"/>
-      <c r="R120" s="59"/>
-      <c r="S120" s="59"/>
+      <c r="M120" s="38"/>
+      <c r="N120" s="38"/>
+      <c r="O120" s="38"/>
+      <c r="P120" s="38"/>
+      <c r="Q120" s="38"/>
+      <c r="R120" s="38"/>
+      <c r="S120" s="38"/>
       <c r="T120" s="38"/>
       <c r="U120" s="39"/>
       <c r="V120" s="40"/>
@@ -8800,54 +8814,54 @@
       <c r="A121" s="35">
         <v>160</v>
       </c>
-      <c r="B121" s="63" t="s">
+      <c r="B121" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C121" s="64" t="s">
+      <c r="C121" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D121" s="63" t="s">
+      <c r="D121" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="E121" s="65" t="s">
+      <c r="E121" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="F121" s="58">
+      <c r="F121" s="37">
         <v>46986</v>
       </c>
-      <c r="G121" s="58" t="s">
+      <c r="G121" s="37" t="s">
         <v>490</v>
       </c>
-      <c r="H121" s="58" t="s">
+      <c r="H121" s="37" t="s">
         <v>491</v>
       </c>
-      <c r="I121" s="60" t="s">
+      <c r="I121" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="J121" s="59" t="s">
+      <c r="J121" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K121" s="59"/>
-      <c r="L121" s="59"/>
-      <c r="M121" s="59" t="s">
+      <c r="K121" s="38"/>
+      <c r="L121" s="38"/>
+      <c r="M121" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N121" s="59" t="s">
+      <c r="N121" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O121" s="59" t="s">
+      <c r="O121" s="38" t="s">
         <v>460</v>
       </c>
-      <c r="P121" s="59" t="s">
+      <c r="P121" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q121" s="59" t="s">
+      <c r="Q121" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R121" s="59" t="s">
+      <c r="R121" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S121" s="59" t="s">
+      <c r="S121" s="38" t="s">
         <v>461</v>
       </c>
       <c r="T121" s="38"/>
@@ -8861,38 +8875,38 @@
       <c r="A122" s="35">
         <v>161</v>
       </c>
-      <c r="B122" s="63" t="s">
+      <c r="B122" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C122" s="64" t="s">
+      <c r="C122" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D122" s="63" t="s">
+      <c r="D122" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="E122" s="65" t="s">
+      <c r="E122" s="49" t="s">
         <v>275</v>
       </c>
-      <c r="F122" s="58"/>
-      <c r="G122" s="58"/>
-      <c r="H122" s="58"/>
-      <c r="I122" s="60"/>
-      <c r="J122" s="59" t="s">
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="42"/>
+      <c r="J122" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K122" s="59" t="s">
+      <c r="K122" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L122" s="59" t="s">
+      <c r="L122" s="38" t="s">
         <v>462</v>
       </c>
-      <c r="M122" s="59"/>
-      <c r="N122" s="59"/>
-      <c r="O122" s="59"/>
-      <c r="P122" s="59"/>
-      <c r="Q122" s="59"/>
-      <c r="R122" s="59"/>
-      <c r="S122" s="59"/>
+      <c r="M122" s="38"/>
+      <c r="N122" s="38"/>
+      <c r="O122" s="38"/>
+      <c r="P122" s="38"/>
+      <c r="Q122" s="38"/>
+      <c r="R122" s="38"/>
+      <c r="S122" s="38"/>
       <c r="T122" s="38"/>
       <c r="U122" s="39"/>
       <c r="V122" s="40"/>
@@ -8904,38 +8918,38 @@
       <c r="A123" s="35">
         <v>162</v>
       </c>
-      <c r="B123" s="63" t="s">
+      <c r="B123" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C123" s="64" t="s">
+      <c r="C123" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D123" s="63" t="s">
+      <c r="D123" s="47" t="s">
         <v>192</v>
       </c>
-      <c r="E123" s="65" t="s">
+      <c r="E123" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="F123" s="58"/>
-      <c r="G123" s="58"/>
-      <c r="H123" s="58"/>
-      <c r="I123" s="60"/>
-      <c r="J123" s="59" t="s">
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="42"/>
+      <c r="J123" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K123" s="59" t="s">
+      <c r="K123" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L123" s="59" t="s">
+      <c r="L123" s="38" t="s">
         <v>493</v>
       </c>
-      <c r="M123" s="59"/>
-      <c r="N123" s="59"/>
-      <c r="O123" s="59"/>
-      <c r="P123" s="59"/>
-      <c r="Q123" s="59"/>
-      <c r="R123" s="59"/>
-      <c r="S123" s="59"/>
+      <c r="M123" s="38"/>
+      <c r="N123" s="38"/>
+      <c r="O123" s="38"/>
+      <c r="P123" s="38"/>
+      <c r="Q123" s="38"/>
+      <c r="R123" s="38"/>
+      <c r="S123" s="38"/>
       <c r="T123" s="38"/>
       <c r="U123" s="39"/>
       <c r="V123" s="40"/>
@@ -8947,54 +8961,54 @@
       <c r="A124" s="35">
         <v>163</v>
       </c>
-      <c r="B124" s="63" t="s">
+      <c r="B124" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C124" s="64" t="s">
+      <c r="C124" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D124" s="63" t="s">
+      <c r="D124" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="E124" s="65" t="s">
+      <c r="E124" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="F124" s="58">
+      <c r="F124" s="37">
         <v>45890</v>
       </c>
-      <c r="G124" s="58" t="s">
+      <c r="G124" s="37" t="s">
         <v>494</v>
       </c>
-      <c r="H124" s="58" t="s">
+      <c r="H124" s="37" t="s">
         <v>495</v>
       </c>
-      <c r="I124" s="60" t="s">
+      <c r="I124" s="42" t="s">
         <v>496</v>
       </c>
-      <c r="J124" s="59" t="s">
+      <c r="J124" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K124" s="59"/>
-      <c r="L124" s="59"/>
-      <c r="M124" s="59" t="s">
+      <c r="K124" s="38"/>
+      <c r="L124" s="38"/>
+      <c r="M124" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N124" s="59" t="s">
+      <c r="N124" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O124" s="59" t="s">
+      <c r="O124" s="38" t="s">
         <v>497</v>
       </c>
-      <c r="P124" s="59" t="s">
+      <c r="P124" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q124" s="59" t="s">
+      <c r="Q124" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R124" s="59" t="s">
+      <c r="R124" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S124" s="59" t="s">
+      <c r="S124" s="38" t="s">
         <v>498</v>
       </c>
       <c r="T124" s="38"/>
@@ -9008,38 +9022,38 @@
       <c r="A125" s="35">
         <v>164</v>
       </c>
-      <c r="B125" s="63" t="s">
+      <c r="B125" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C125" s="64" t="s">
+      <c r="C125" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D125" s="63" t="s">
+      <c r="D125" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="E125" s="65" t="s">
+      <c r="E125" s="49" t="s">
         <v>278</v>
       </c>
-      <c r="F125" s="58"/>
-      <c r="G125" s="58"/>
-      <c r="H125" s="58"/>
-      <c r="I125" s="60"/>
-      <c r="J125" s="59" t="s">
+      <c r="F125" s="37"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="37"/>
+      <c r="I125" s="42"/>
+      <c r="J125" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K125" s="59" t="s">
+      <c r="K125" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L125" s="59" t="s">
+      <c r="L125" s="38" t="s">
         <v>499</v>
       </c>
-      <c r="M125" s="59"/>
-      <c r="N125" s="59"/>
-      <c r="O125" s="59"/>
-      <c r="P125" s="59"/>
-      <c r="Q125" s="59"/>
-      <c r="R125" s="59"/>
-      <c r="S125" s="59"/>
+      <c r="M125" s="38"/>
+      <c r="N125" s="38"/>
+      <c r="O125" s="38"/>
+      <c r="P125" s="38"/>
+      <c r="Q125" s="38"/>
+      <c r="R125" s="38"/>
+      <c r="S125" s="38"/>
       <c r="T125" s="38"/>
       <c r="U125" s="39"/>
       <c r="V125" s="40"/>
@@ -9051,54 +9065,54 @@
       <c r="A126" s="35">
         <v>165</v>
       </c>
-      <c r="B126" s="63" t="s">
+      <c r="B126" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C126" s="64" t="s">
+      <c r="C126" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D126" s="63" t="s">
+      <c r="D126" s="47" t="s">
         <v>195</v>
       </c>
-      <c r="E126" s="65" t="s">
+      <c r="E126" s="49" t="s">
         <v>279</v>
       </c>
-      <c r="F126" s="58">
+      <c r="F126" s="37">
         <v>45890</v>
       </c>
-      <c r="G126" s="58" t="s">
+      <c r="G126" s="37" t="s">
         <v>500</v>
       </c>
-      <c r="H126" s="58" t="s">
+      <c r="H126" s="37" t="s">
         <v>501</v>
       </c>
-      <c r="I126" s="60" t="s">
+      <c r="I126" s="42" t="s">
         <v>502</v>
       </c>
-      <c r="J126" s="59" t="s">
+      <c r="J126" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K126" s="59"/>
-      <c r="L126" s="59"/>
-      <c r="M126" s="59" t="s">
+      <c r="K126" s="38"/>
+      <c r="L126" s="38"/>
+      <c r="M126" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N126" s="59" t="s">
+      <c r="N126" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O126" s="59" t="s">
+      <c r="O126" s="38" t="s">
         <v>503</v>
       </c>
-      <c r="P126" s="59" t="s">
+      <c r="P126" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q126" s="59" t="s">
+      <c r="Q126" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R126" s="59" t="s">
+      <c r="R126" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S126" s="59" t="s">
+      <c r="S126" s="38" t="s">
         <v>470</v>
       </c>
       <c r="T126" s="38"/>
@@ -9112,54 +9126,54 @@
       <c r="A127" s="35">
         <v>166</v>
       </c>
-      <c r="B127" s="63" t="s">
+      <c r="B127" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C127" s="64" t="s">
+      <c r="C127" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D127" s="63" t="s">
+      <c r="D127" s="47" t="s">
         <v>196</v>
       </c>
-      <c r="E127" s="65" t="s">
+      <c r="E127" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="F127" s="58">
+      <c r="F127" s="37">
         <v>45911</v>
       </c>
-      <c r="G127" s="58" t="s">
+      <c r="G127" s="37" t="s">
         <v>504</v>
       </c>
-      <c r="H127" s="58" t="s">
+      <c r="H127" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="I127" s="60" t="s">
+      <c r="I127" s="42" t="s">
         <v>506</v>
       </c>
-      <c r="J127" s="59" t="s">
+      <c r="J127" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K127" s="59"/>
-      <c r="L127" s="59"/>
-      <c r="M127" s="59" t="s">
+      <c r="K127" s="38"/>
+      <c r="L127" s="38"/>
+      <c r="M127" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N127" s="59" t="s">
+      <c r="N127" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O127" s="59" t="s">
+      <c r="O127" s="38" t="s">
         <v>474</v>
       </c>
-      <c r="P127" s="59" t="s">
+      <c r="P127" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q127" s="59" t="s">
+      <c r="Q127" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R127" s="59" t="s">
+      <c r="R127" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S127" s="59" t="s">
+      <c r="S127" s="38" t="s">
         <v>461</v>
       </c>
       <c r="T127" s="38"/>
@@ -9173,38 +9187,38 @@
       <c r="A128" s="35">
         <v>167</v>
       </c>
-      <c r="B128" s="63" t="s">
+      <c r="B128" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C128" s="64" t="s">
+      <c r="C128" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D128" s="63" t="s">
+      <c r="D128" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="E128" s="65" t="s">
+      <c r="E128" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="F128" s="58"/>
-      <c r="G128" s="58"/>
-      <c r="H128" s="58"/>
-      <c r="I128" s="60"/>
-      <c r="J128" s="59" t="s">
+      <c r="F128" s="37"/>
+      <c r="G128" s="37"/>
+      <c r="H128" s="37"/>
+      <c r="I128" s="42"/>
+      <c r="J128" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K128" s="59" t="s">
+      <c r="K128" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L128" s="59" t="s">
+      <c r="L128" s="38" t="s">
         <v>475</v>
       </c>
-      <c r="M128" s="59"/>
-      <c r="N128" s="59"/>
-      <c r="O128" s="59"/>
-      <c r="P128" s="59"/>
-      <c r="Q128" s="59"/>
-      <c r="R128" s="59"/>
-      <c r="S128" s="59"/>
+      <c r="M128" s="38"/>
+      <c r="N128" s="38"/>
+      <c r="O128" s="38"/>
+      <c r="P128" s="38"/>
+      <c r="Q128" s="38"/>
+      <c r="R128" s="38"/>
+      <c r="S128" s="38"/>
       <c r="T128" s="38"/>
       <c r="U128" s="39"/>
       <c r="V128" s="40"/>
@@ -9216,54 +9230,54 @@
       <c r="A129" s="35">
         <v>168</v>
       </c>
-      <c r="B129" s="63" t="s">
+      <c r="B129" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C129" s="64" t="s">
+      <c r="C129" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D129" s="63" t="s">
+      <c r="D129" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="E129" s="65" t="s">
+      <c r="E129" s="49" t="s">
         <v>282</v>
       </c>
-      <c r="F129" s="58">
+      <c r="F129" s="37">
         <v>45911</v>
       </c>
-      <c r="G129" s="58" t="s">
+      <c r="G129" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="H129" s="58" t="s">
+      <c r="H129" s="37" t="s">
         <v>508</v>
       </c>
-      <c r="I129" s="60" t="s">
+      <c r="I129" s="42" t="s">
         <v>509</v>
       </c>
-      <c r="J129" s="59" t="s">
+      <c r="J129" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K129" s="59"/>
-      <c r="L129" s="59"/>
-      <c r="M129" s="59" t="s">
+      <c r="K129" s="38"/>
+      <c r="L129" s="38"/>
+      <c r="M129" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N129" s="59" t="s">
+      <c r="N129" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O129" s="59" t="s">
+      <c r="O129" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="P129" s="59" t="s">
+      <c r="P129" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q129" s="59" t="s">
+      <c r="Q129" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R129" s="59" t="s">
+      <c r="R129" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S129" s="59" t="s">
+      <c r="S129" s="38" t="s">
         <v>480</v>
       </c>
       <c r="T129" s="38"/>
@@ -9277,38 +9291,38 @@
       <c r="A130" s="35">
         <v>169</v>
       </c>
-      <c r="B130" s="63" t="s">
+      <c r="B130" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C130" s="64" t="s">
+      <c r="C130" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D130" s="63" t="s">
+      <c r="D130" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="E130" s="65" t="s">
+      <c r="E130" s="49" t="s">
         <v>284</v>
       </c>
-      <c r="F130" s="58"/>
-      <c r="G130" s="58"/>
-      <c r="H130" s="58"/>
-      <c r="I130" s="60"/>
-      <c r="J130" s="59" t="s">
+      <c r="F130" s="37"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="37"/>
+      <c r="I130" s="42"/>
+      <c r="J130" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K130" s="59" t="s">
+      <c r="K130" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L130" s="59" t="s">
+      <c r="L130" s="38" t="s">
         <v>510</v>
       </c>
-      <c r="M130" s="59"/>
-      <c r="N130" s="59"/>
-      <c r="O130" s="59"/>
-      <c r="P130" s="59"/>
-      <c r="Q130" s="59"/>
-      <c r="R130" s="59"/>
-      <c r="S130" s="59"/>
+      <c r="M130" s="38"/>
+      <c r="N130" s="38"/>
+      <c r="O130" s="38"/>
+      <c r="P130" s="38"/>
+      <c r="Q130" s="38"/>
+      <c r="R130" s="38"/>
+      <c r="S130" s="38"/>
       <c r="T130" s="38"/>
       <c r="U130" s="39"/>
       <c r="V130" s="40"/>
@@ -10612,45 +10626,45 @@
       </c>
     </row>
     <row r="166" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="61">
+      <c r="A166" s="45">
         <v>448</v>
       </c>
-      <c r="B166" s="63" t="s">
+      <c r="B166" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C166" s="64" t="s">
+      <c r="C166" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D166" s="63" t="s">
+      <c r="D166" s="47" t="s">
         <v>382</v>
       </c>
-      <c r="E166" s="65" t="s">
+      <c r="E166" s="49" t="s">
         <v>384</v>
       </c>
-      <c r="F166" s="58">
+      <c r="F166" s="37">
         <v>45890</v>
       </c>
-      <c r="G166" s="58" t="s">
+      <c r="G166" s="37" t="s">
         <v>511</v>
       </c>
-      <c r="H166" s="58" t="s">
+      <c r="H166" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="I166" s="60" t="s">
+      <c r="I166" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="J166" s="59" t="s">
+      <c r="J166" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K166" s="59"/>
-      <c r="L166" s="59"/>
-      <c r="M166" s="59"/>
-      <c r="N166" s="59"/>
-      <c r="O166" s="59"/>
-      <c r="P166" s="59"/>
-      <c r="Q166" s="59"/>
-      <c r="R166" s="59"/>
-      <c r="S166" s="59"/>
+      <c r="K166" s="38"/>
+      <c r="L166" s="38"/>
+      <c r="M166" s="38"/>
+      <c r="N166" s="38"/>
+      <c r="O166" s="38"/>
+      <c r="P166" s="38"/>
+      <c r="Q166" s="38"/>
+      <c r="R166" s="38"/>
+      <c r="S166" s="38"/>
       <c r="T166" s="38"/>
       <c r="U166" s="39"/>
       <c r="V166" s="40"/>
@@ -10662,36 +10676,36 @@
       <c r="A167" s="35">
         <v>449</v>
       </c>
-      <c r="B167" s="63" t="s">
+      <c r="B167" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C167" s="64" t="s">
+      <c r="C167" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D167" s="63" t="s">
+      <c r="D167" s="47" t="s">
         <v>383</v>
       </c>
-      <c r="E167" s="65" t="s">
+      <c r="E167" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="F167" s="58"/>
-      <c r="G167" s="58"/>
-      <c r="H167" s="58"/>
-      <c r="I167" s="60"/>
-      <c r="J167" s="59" t="s">
+      <c r="F167" s="37"/>
+      <c r="G167" s="37"/>
+      <c r="H167" s="37"/>
+      <c r="I167" s="42"/>
+      <c r="J167" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K167" s="59" t="s">
+      <c r="K167" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="L167" s="59"/>
-      <c r="M167" s="59"/>
-      <c r="N167" s="59"/>
-      <c r="O167" s="59"/>
-      <c r="P167" s="59"/>
-      <c r="Q167" s="59"/>
-      <c r="R167" s="59"/>
-      <c r="S167" s="59"/>
+      <c r="L167" s="38"/>
+      <c r="M167" s="38"/>
+      <c r="N167" s="38"/>
+      <c r="O167" s="38"/>
+      <c r="P167" s="38"/>
+      <c r="Q167" s="38"/>
+      <c r="R167" s="38"/>
+      <c r="S167" s="38"/>
       <c r="T167" s="38"/>
       <c r="U167" s="39"/>
       <c r="V167" s="40"/>
@@ -11073,54 +11087,54 @@
       <c r="A178" s="35">
         <v>461</v>
       </c>
-      <c r="B178" s="63" t="s">
+      <c r="B178" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C178" s="64" t="s">
+      <c r="C178" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D178" s="63" t="s">
+      <c r="D178" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="E178" s="65" t="s">
+      <c r="E178" s="49" t="s">
         <v>386</v>
       </c>
-      <c r="F178" s="62">
+      <c r="F178" s="46">
         <v>45911</v>
       </c>
-      <c r="G178" s="57" t="s">
+      <c r="G178" s="35" t="s">
         <v>514</v>
       </c>
-      <c r="H178" s="57" t="s">
+      <c r="H178" s="35" t="s">
         <v>515</v>
       </c>
-      <c r="I178" s="57" t="s">
+      <c r="I178" s="35" t="s">
         <v>516</v>
       </c>
-      <c r="J178" s="59" t="s">
+      <c r="J178" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K178" s="59"/>
-      <c r="L178" s="57"/>
-      <c r="M178" s="59" t="s">
+      <c r="K178" s="38"/>
+      <c r="L178" s="35"/>
+      <c r="M178" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N178" s="59" t="s">
+      <c r="N178" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O178" s="59" t="s">
+      <c r="O178" s="38" t="s">
         <v>517</v>
       </c>
-      <c r="P178" s="59" t="s">
+      <c r="P178" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q178" s="59" t="s">
+      <c r="Q178" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="R178" s="59" t="s">
+      <c r="R178" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="S178" s="59" t="s">
+      <c r="S178" s="38" t="s">
         <v>480</v>
       </c>
       <c r="T178" s="38"/>
@@ -11134,38 +11148,38 @@
       <c r="A179" s="35">
         <v>462</v>
       </c>
-      <c r="B179" s="63" t="s">
+      <c r="B179" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C179" s="64" t="s">
+      <c r="C179" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D179" s="63" t="s">
+      <c r="D179" s="47" t="s">
         <v>390</v>
       </c>
-      <c r="E179" s="65" t="s">
+      <c r="E179" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="F179" s="57"/>
-      <c r="G179" s="57"/>
-      <c r="H179" s="57"/>
-      <c r="I179" s="57"/>
-      <c r="J179" s="59" t="s">
+      <c r="F179" s="35"/>
+      <c r="G179" s="35"/>
+      <c r="H179" s="35"/>
+      <c r="I179" s="35"/>
+      <c r="J179" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K179" s="59" t="s">
+      <c r="K179" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L179" s="59" t="s">
+      <c r="L179" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="M179" s="59"/>
-      <c r="N179" s="59"/>
-      <c r="O179" s="57"/>
-      <c r="P179" s="59"/>
-      <c r="Q179" s="59"/>
-      <c r="R179" s="59"/>
-      <c r="S179" s="57"/>
+      <c r="M179" s="38"/>
+      <c r="N179" s="38"/>
+      <c r="O179" s="35"/>
+      <c r="P179" s="38"/>
+      <c r="Q179" s="38"/>
+      <c r="R179" s="38"/>
+      <c r="S179" s="35"/>
       <c r="T179" s="38"/>
       <c r="U179" s="35"/>
       <c r="V179" s="35"/>
@@ -11173,7 +11187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>463</v>
       </c>
@@ -11362,38 +11376,38 @@
       <c r="A185" s="35">
         <v>468</v>
       </c>
-      <c r="B185" s="63" t="s">
+      <c r="B185" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C185" s="64" t="s">
+      <c r="C185" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D185" s="63" t="s">
+      <c r="D185" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="E185" s="65" t="s">
+      <c r="E185" s="49" t="s">
         <v>401</v>
       </c>
-      <c r="F185" s="62"/>
-      <c r="G185" s="57"/>
-      <c r="H185" s="57"/>
-      <c r="I185" s="57"/>
-      <c r="J185" s="59" t="s">
+      <c r="F185" s="46"/>
+      <c r="G185" s="35"/>
+      <c r="H185" s="35"/>
+      <c r="I185" s="35"/>
+      <c r="J185" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K185" s="59" t="s">
+      <c r="K185" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L185" s="59" t="s">
+      <c r="L185" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="M185" s="59"/>
-      <c r="N185" s="59"/>
-      <c r="O185" s="57"/>
-      <c r="P185" s="59"/>
-      <c r="Q185" s="59"/>
-      <c r="R185" s="59"/>
-      <c r="S185" s="57"/>
+      <c r="M185" s="38"/>
+      <c r="N185" s="38"/>
+      <c r="O185" s="35"/>
+      <c r="P185" s="38"/>
+      <c r="Q185" s="38"/>
+      <c r="R185" s="38"/>
+      <c r="S185" s="35"/>
       <c r="T185" s="38"/>
       <c r="U185" s="35"/>
       <c r="V185" s="35"/>
@@ -11476,45 +11490,45 @@
       </c>
     </row>
     <row r="188" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="61">
+      <c r="A188" s="45">
         <v>471</v>
       </c>
-      <c r="B188" s="63" t="s">
+      <c r="B188" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C188" s="64" t="s">
+      <c r="C188" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D188" s="63" t="s">
+      <c r="D188" s="47" t="s">
         <v>414</v>
       </c>
-      <c r="E188" s="65" t="s">
+      <c r="E188" s="49" t="s">
         <v>415</v>
       </c>
-      <c r="F188" s="58">
+      <c r="F188" s="37">
         <v>45890</v>
       </c>
-      <c r="G188" s="58" t="s">
+      <c r="G188" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="H188" s="58" t="s">
+      <c r="H188" s="37" t="s">
         <v>484</v>
       </c>
-      <c r="I188" s="60" t="s">
+      <c r="I188" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="J188" s="59" t="s">
+      <c r="J188" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K188" s="59"/>
-      <c r="L188" s="59"/>
-      <c r="M188" s="59"/>
-      <c r="N188" s="59"/>
-      <c r="O188" s="59"/>
-      <c r="P188" s="59"/>
-      <c r="Q188" s="59"/>
-      <c r="R188" s="59"/>
-      <c r="S188" s="59"/>
+      <c r="K188" s="38"/>
+      <c r="L188" s="38"/>
+      <c r="M188" s="38"/>
+      <c r="N188" s="38"/>
+      <c r="O188" s="38"/>
+      <c r="P188" s="38"/>
+      <c r="Q188" s="38"/>
+      <c r="R188" s="38"/>
+      <c r="S188" s="38"/>
       <c r="T188" s="38"/>
       <c r="U188" s="39"/>
       <c r="V188" s="40"/>
@@ -11526,36 +11540,36 @@
       <c r="A189" s="35">
         <v>472</v>
       </c>
-      <c r="B189" s="63" t="s">
+      <c r="B189" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C189" s="64" t="s">
+      <c r="C189" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D189" s="63" t="s">
+      <c r="D189" s="47" t="s">
         <v>419</v>
       </c>
-      <c r="E189" s="65" t="s">
+      <c r="E189" s="49" t="s">
         <v>420</v>
       </c>
-      <c r="F189" s="58"/>
-      <c r="G189" s="58"/>
-      <c r="H189" s="58"/>
-      <c r="I189" s="60"/>
-      <c r="J189" s="59" t="s">
+      <c r="F189" s="37"/>
+      <c r="G189" s="37"/>
+      <c r="H189" s="37"/>
+      <c r="I189" s="42"/>
+      <c r="J189" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K189" s="59" t="s">
+      <c r="K189" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="L189" s="59"/>
-      <c r="M189" s="59"/>
-      <c r="N189" s="59"/>
-      <c r="O189" s="59"/>
-      <c r="P189" s="59"/>
-      <c r="Q189" s="59"/>
-      <c r="R189" s="59"/>
-      <c r="S189" s="59"/>
+      <c r="L189" s="38"/>
+      <c r="M189" s="38"/>
+      <c r="N189" s="38"/>
+      <c r="O189" s="38"/>
+      <c r="P189" s="38"/>
+      <c r="Q189" s="38"/>
+      <c r="R189" s="38"/>
+      <c r="S189" s="38"/>
       <c r="T189" s="38"/>
       <c r="U189" s="39"/>
       <c r="V189" s="40"/>
@@ -11604,36 +11618,36 @@
       <c r="A191" s="35">
         <v>474</v>
       </c>
-      <c r="B191" s="63" t="s">
+      <c r="B191" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C191" s="64" t="s">
+      <c r="C191" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D191" s="63" t="s">
+      <c r="D191" s="47" t="s">
         <v>423</v>
       </c>
-      <c r="E191" s="65" t="s">
+      <c r="E191" s="49" t="s">
         <v>426</v>
       </c>
-      <c r="F191" s="58"/>
-      <c r="G191" s="58"/>
-      <c r="H191" s="58"/>
-      <c r="I191" s="60"/>
-      <c r="J191" s="59" t="s">
+      <c r="F191" s="37"/>
+      <c r="G191" s="37"/>
+      <c r="H191" s="37"/>
+      <c r="I191" s="42"/>
+      <c r="J191" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K191" s="59" t="s">
+      <c r="K191" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="L191" s="59"/>
-      <c r="M191" s="59"/>
-      <c r="N191" s="59"/>
-      <c r="O191" s="59"/>
-      <c r="P191" s="59"/>
-      <c r="Q191" s="59"/>
-      <c r="R191" s="59"/>
-      <c r="S191" s="59"/>
+      <c r="L191" s="38"/>
+      <c r="M191" s="38"/>
+      <c r="N191" s="38"/>
+      <c r="O191" s="38"/>
+      <c r="P191" s="38"/>
+      <c r="Q191" s="38"/>
+      <c r="R191" s="38"/>
+      <c r="S191" s="38"/>
       <c r="T191" s="38"/>
       <c r="U191" s="39"/>
       <c r="V191" s="40"/>
@@ -11645,36 +11659,36 @@
       <c r="A192" s="35">
         <v>475</v>
       </c>
-      <c r="B192" s="63" t="s">
+      <c r="B192" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C192" s="64" t="s">
+      <c r="C192" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D192" s="63" t="s">
+      <c r="D192" s="47" t="s">
         <v>422</v>
       </c>
-      <c r="E192" s="65" t="s">
+      <c r="E192" s="49" t="s">
         <v>427</v>
       </c>
-      <c r="F192" s="58"/>
-      <c r="G192" s="58"/>
-      <c r="H192" s="58"/>
-      <c r="I192" s="60"/>
-      <c r="J192" s="59" t="s">
+      <c r="F192" s="37"/>
+      <c r="G192" s="37"/>
+      <c r="H192" s="37"/>
+      <c r="I192" s="42"/>
+      <c r="J192" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="K192" s="59" t="s">
+      <c r="K192" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="L192" s="59"/>
-      <c r="M192" s="59"/>
-      <c r="N192" s="59"/>
-      <c r="O192" s="59"/>
-      <c r="P192" s="59"/>
-      <c r="Q192" s="59"/>
-      <c r="R192" s="59"/>
-      <c r="S192" s="59"/>
+      <c r="L192" s="38"/>
+      <c r="M192" s="38"/>
+      <c r="N192" s="38"/>
+      <c r="O192" s="38"/>
+      <c r="P192" s="38"/>
+      <c r="Q192" s="38"/>
+      <c r="R192" s="38"/>
+      <c r="S192" s="38"/>
       <c r="T192" s="38"/>
       <c r="U192" s="39"/>
       <c r="V192" s="40"/>
@@ -17990,6 +18004,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -18247,28 +18282,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18287,31 +18326,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>